<commit_message>
Remove n_news=1000; update xlsx for n_news=1250
</commit_message>
<xml_diff>
--- a/results/accuracy.xlsx
+++ b/results/accuracy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\git\TCC-80true20fake\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4584960D-3D2B-46A0-8F69-EDA29BB5BA97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293AAA9C-6DE3-45E8-A115-0A647A204CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30795" yWindow="3045" windowWidth="12885" windowHeight="11385" xr2:uid="{15A971EA-431C-4990-A4C6-5F929271826D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{15A971EA-431C-4990-A4C6-5F929271826D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>EE</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>LOF</t>
-  </si>
-  <si>
-    <t>Modelo</t>
   </si>
 </sst>
 </file>
@@ -67,12 +64,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -107,14 +110,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -303,7 +306,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1250</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2500</c:v>
@@ -327,7 +330,7 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.72099999999999997</c:v>
+                  <c:v>0.70240000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.71040000000000003</c:v>
@@ -439,7 +442,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1250</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2500</c:v>
@@ -463,7 +466,7 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.80300000000000005</c:v>
+                  <c:v>0.8024</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.8024</c:v>
@@ -575,7 +578,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1250</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2500</c:v>
@@ -599,7 +602,7 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.80700000000000005</c:v>
+                  <c:v>0.80320000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.8024</c:v>
@@ -711,7 +714,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>1250</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2500</c:v>
@@ -735,7 +738,7 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.84299999999999997</c:v>
+                  <c:v>0.85199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.83599999999999997</c:v>
@@ -1950,46 +1953,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1D63C6-1D98-47AF-9794-433DA7D7CAA5}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C1" s="1">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3">
+        <v>1250</v>
+      </c>
+      <c r="C1" s="3">
         <v>2500</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="3">
         <v>5000</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="3">
         <v>10000</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="3">
         <v>20000</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
-        <v>0.72099999999999997</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2" s="2">
+        <v>0.70240000000000002</v>
+      </c>
+      <c r="C2" s="2">
         <v>0.71040000000000003</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>0.71499999999999997</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>0.74399999999999999</v>
       </c>
       <c r="F2" s="1">
@@ -1997,19 +1996,19 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
-        <v>0.80300000000000005</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3" s="2">
         <v>0.8024</v>
       </c>
-      <c r="D3" s="3">
+      <c r="C3" s="2">
+        <v>0.8024</v>
+      </c>
+      <c r="D3" s="2">
         <v>0.80079999999999996</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>0.8004</v>
       </c>
       <c r="F3" s="1">
@@ -2017,19 +2016,19 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>0.80700000000000005</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="2">
+        <v>0.80320000000000003</v>
+      </c>
+      <c r="C4" s="2">
         <v>0.8024</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>0.8024</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.80269999999999997</v>
       </c>
       <c r="F4" s="1">
@@ -2037,19 +2036,19 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
-        <v>0.84299999999999997</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5" s="2">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="C5" s="2">
         <v>0.83599999999999997</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>0.82679999999999998</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>0.85660000000000003</v>
       </c>
       <c r="F5" s="1">

</xml_diff>